<commit_message>
explode sku unit on import
</commit_message>
<xml_diff>
--- a/public/assets/FokusMDImport.xlsx
+++ b/public/assets/FokusMDImport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sasa_mtcgtc\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>product</t>
   </si>
@@ -36,22 +36,25 @@
     <t>product1</t>
   </si>
   <si>
-    <t>wew112</t>
-  </si>
-  <si>
-    <t>wew2</t>
-  </si>
-  <si>
     <t>sku</t>
   </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>aw12, aw45</t>
-  </si>
-  <si>
-    <t>Fast Moving</t>
+    <t>value</t>
+  </si>
+  <si>
+    <t>sub1</t>
+  </si>
+  <si>
+    <t>cat1</t>
+  </si>
+  <si>
+    <t>skus1,skus2</t>
+  </si>
+  <si>
+    <t>fast moving</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -389,7 +392,7 @@
     <col min="1" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,13 +406,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -417,16 +423,19 @@
         <v>12345</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>